<commit_message>
user guide for co2mpas driver model
</commit_message>
<xml_diff>
--- a/build/lib/co2mpas_driver/template/sample.xlsx
+++ b/build/lib/co2mpas_driver/template/sample.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apps\new_MFC\co2mpas_driver\template\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9435" activeTab="3"/>
   </bookViews>
@@ -18,8 +13,8 @@
     <sheet name="time_series" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -172,17 +167,17 @@
     </r>
   </si>
   <si>
-    <t>v_start</t>
-  </si>
-  <si>
     <t>Current speed</t>
+  </si>
+  <si>
+    <t>starting_speed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,7 +281,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -321,7 +316,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -498,27 +493,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -529,7 +524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -540,7 +535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -551,15 +546,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -568,21 +563,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
     <col min="3" max="3" width="58.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -590,7 +585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -608,20 +603,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -629,7 +624,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -644,16 +639,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -667,172 +662,129 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <f xml:space="preserve"> A2 + 1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <f t="shared" ref="A4:A22" si="0" xml:space="preserve"> A3 + 1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22">
+        <f t="shared" si="0"/>
         <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22">
-        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Jupyter notebook used as an interface for users to use co2mpas driver library
</commit_message>
<xml_diff>
--- a/build/lib/co2mpas_driver/template/sample.xlsx
+++ b/build/lib/co2mpas_driver/template/sample.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apps\new_MFC\co2mpas_driver\template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9435" activeTab="3"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9435"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="2" r:id="rId1"/>
@@ -12,9 +17,9 @@
     <sheet name="vehicle_inputs" sheetId="3" r:id="rId3"/>
     <sheet name="time_series" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -176,8 +181,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,7 +286,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -316,7 +321,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -493,27 +498,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -524,18 +529,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -546,7 +551,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -563,21 +568,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
     <col min="3" max="3" width="58.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -585,12 +590,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>35135</v>
+        <v>39393</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -603,20 +608,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -624,7 +629,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -639,16 +644,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -662,129 +667,212 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <f xml:space="preserve"> A2 + 1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="B3">
+        <f>B2 + 5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A22" si="0" xml:space="preserve"> A3 + 1</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="B4">
+        <f t="shared" ref="B4:B22" si="1">B3 + 5</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="B5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>